<commit_message>
updating piping input excel
</commit_message>
<xml_diff>
--- a/Piping input.xlsx
+++ b/Piping input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iNeuron\Civil_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1D63A8-D8D9-4267-B1A3-4974BD4B7016}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BB6C52-D54E-4EEE-8BBD-E5653D1FFA22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Line no.</t>
   </si>
@@ -155,14 +155,14 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,11 +443,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,39 +457,39 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="4"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>4</v>
       </c>
     </row>
@@ -516,6 +516,32 @@
         <v>0</v>
       </c>
       <c r="H3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>101</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>28</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
         <v>0.3</v>
       </c>
     </row>

</xml_diff>